<commit_message>
Updated Sylubus and Schedule
</commit_message>
<xml_diff>
--- a/AGGP247_Schedule_S20.xlsx
+++ b/AGGP247_Schedule_S20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\AGGP247c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875186EB-8B6D-4ED5-BDA3-9B088D04507F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEB086D-268C-4373-8F65-C4A6ED8BE4DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>M</t>
   </si>
@@ -72,18 +72,12 @@
     <t>Lab 1 DUE</t>
   </si>
   <si>
-    <t>Circle 1</t>
-  </si>
-  <si>
     <t>Elipse</t>
   </si>
   <si>
     <t>Triangle collison</t>
   </si>
   <si>
-    <t>Lab 2 DUE</t>
-  </si>
-  <si>
     <t>Lab 3 Due</t>
   </si>
   <si>
@@ -105,7 +99,16 @@
     <t>Finals Week</t>
   </si>
   <si>
-    <t>Gravity  &amp; Forces</t>
+    <t>Circles</t>
+  </si>
+  <si>
+    <t>No Class 17th, Lab 2 DUE</t>
+  </si>
+  <si>
+    <t>Project Review</t>
+  </si>
+  <si>
+    <t>Gravity &amp; Forces</t>
   </si>
 </sst>
 </file>
@@ -799,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,6 +1031,7 @@
         <v>14</v>
       </c>
       <c r="L6" s="17"/>
+      <c r="M6" s="21"/>
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1035,7 +1039,7 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="42">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -1064,11 +1068,11 @@
       </c>
       <c r="J7" s="33"/>
       <c r="K7" s="20" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="21" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="O7" s="10"/>
     </row>
@@ -1106,7 +1110,7 @@
       </c>
       <c r="J8" s="33"/>
       <c r="K8" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" s="21"/>
@@ -1146,11 +1150,11 @@
       </c>
       <c r="J9" s="33"/>
       <c r="K9" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L9" s="17"/>
       <c r="M9" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1187,7 +1191,7 @@
       </c>
       <c r="J10" s="65"/>
       <c r="K10" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
@@ -1265,11 +1269,11 @@
       </c>
       <c r="J12" s="33"/>
       <c r="K12" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L12" s="17"/>
       <c r="M12" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1306,7 +1310,7 @@
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
@@ -1345,11 +1349,11 @@
       </c>
       <c r="J14" s="33"/>
       <c r="K14" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1386,10 +1390,10 @@
       </c>
       <c r="J15" s="33"/>
       <c r="K15" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L15" s="17"/>
-      <c r="M15" s="18"/>
+      <c r="M15" s="21"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="str">
@@ -1425,10 +1429,12 @@
       </c>
       <c r="J16" s="33"/>
       <c r="K16" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L16" s="17"/>
-      <c r="M16" s="18"/>
+      <c r="M16" s="21" t="s">
+        <v>27</v>
+      </c>
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1465,12 +1471,10 @@
       </c>
       <c r="J17" s="33"/>
       <c r="K17" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L17" s="17"/>
-      <c r="M17" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="M17" s="21"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="str">
@@ -1506,9 +1510,12 @@
       </c>
       <c r="J18" s="33"/>
       <c r="K18" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L18" s="17"/>
+      <c r="M18" s="21" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="str">

</xml_diff>